<commit_message>
move and rescale 2.1x3 barcode
</commit_message>
<xml_diff>
--- a/Packing_Summary_20230109.xlsx
+++ b/Packing_Summary_20230109.xlsx
@@ -139,7 +139,7 @@
     <t>ขนม Weigh</t>
   </si>
   <si>
-    <t>22.7</t>
+    <t>22.69</t>
   </si>
   <si>
     <t>ผลไม้</t>
@@ -1012,7 +1012,7 @@
     <t>Product Weight (Kg)</t>
   </si>
   <si>
-    <t>779.6</t>
+    <t>779.59</t>
   </si>
   <si>
     <t>Carton Weight (Kg)</t>
@@ -1636,7 +1636,7 @@
         <v>15</v>
       </c>
       <c r="F17">
-        <v>5.89</v>
+        <v>5.880000000000001</v>
       </c>
     </row>
     <row r="18" spans="1:6">

</xml_diff>